<commit_message>
2.15 Fix Activation Buttons
</commit_message>
<xml_diff>
--- a/Notes.xlsx
+++ b/Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicus\Documents\AnkeNaratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5D1FC5-AE5B-4441-A477-C02945842416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CA8B87-E3DD-4688-9B3B-3F2E4C0358AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Process</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>PlantUML Complete</t>
+  </si>
+  <si>
+    <t>Fix Activation Buttons</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +111,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,10 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +443,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,23 +466,29 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>